<commit_message>
Update on weekly tracker by khaleel
update
</commit_message>
<xml_diff>
--- a/03_WeeklyTask/WeeklyTracker.xlsx
+++ b/03_WeeklyTask/WeeklyTracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Khaleel" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t xml:space="preserve">Objective CAN</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Khaee1</t>
   </si>
   <si>
-    <t xml:space="preserve">In Progrees </t>
+    <t xml:space="preserve">In Progress </t>
   </si>
   <si>
     <t xml:space="preserve">working on role creation with esp32</t>
@@ -67,6 +67,21 @@
     <t xml:space="preserve">Task 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Currently working on pendios dashboard functionalities with Arun and Rahamath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun, Rahamath and Khaleel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action page is under progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">Task 3</t>
   </si>
   <si>
@@ -101,9 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sunil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Progress </t>
   </si>
   <si>
     <t xml:space="preserve">17-jun</t>
@@ -248,13 +260,13 @@
   </sheetPr>
   <dimension ref="C3:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.42"/>
   </cols>
@@ -324,11 +336,25 @@
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -353,11 +379,11 @@
   </sheetPr>
   <dimension ref="A3:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="10.58"/>
@@ -368,7 +394,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -391,25 +417,25 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,22 +443,22 @@
         <v>44364</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -457,12 +483,12 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.29"/>
@@ -504,16 +530,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +567,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="n">
@@ -566,7 +592,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -589,25 +615,25 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,7 +644,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>